<commit_message>
added AIC results of Prebus_2017
</commit_message>
<xml_diff>
--- a/Tables-Figures/Tables/Tables.xlsx
+++ b/Tables-Figures/Tables/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="460" windowWidth="20360" windowHeight="14760" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="7020" yWindow="460" windowWidth="20360" windowHeight="14760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tab1-datasets" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="SM1-PF-sim" sheetId="3" r:id="rId5"/>
     <sheet name="wds" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -454,7 +454,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -608,6 +608,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -617,67 +650,37 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1188,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -1201,16 +1204,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
@@ -1241,10 +1244,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -1346,10 +1349,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="54"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -1464,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2116,229 +2119,291 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="64"/>
-      <c r="B36" s="64" t="s">
+      <c r="A36" s="53"/>
+      <c r="B36" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="65">
+      <c r="C36" s="54">
         <v>5774753.4500000002</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="54">
         <v>0</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="55">
         <v>496</v>
       </c>
-      <c r="F36" s="66">
+      <c r="F36" s="55">
         <v>5168</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="66">
+      <c r="C37" s="55">
         <v>17672425.579100002</v>
       </c>
-      <c r="D37" s="68">
-        <f>(C$43-C37)</f>
+      <c r="D37" s="57">
+        <f t="shared" ref="D37:D43" si="0">(C$43-C37)</f>
         <v>-336593.90430000052</v>
       </c>
-      <c r="E37" s="66">
+      <c r="E37" s="55">
         <v>1</v>
       </c>
-      <c r="F37" s="66">
+      <c r="F37" s="55">
         <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="67"/>
-      <c r="B38" s="64" t="s">
+      <c r="A38" s="56"/>
+      <c r="B38" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="66">
+      <c r="C38" s="55">
         <v>17591017.273499999</v>
       </c>
-      <c r="D38" s="68">
-        <f>(C$43-C38)</f>
+      <c r="D38" s="57">
+        <f t="shared" si="0"/>
         <v>-255185.59869999811</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="55">
         <v>158</v>
       </c>
-      <c r="F38" s="66">
+      <c r="F38" s="55">
         <v>1950</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="67"/>
-      <c r="B39" s="64" t="s">
+      <c r="A39" s="56"/>
+      <c r="B39" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="66">
+      <c r="C39" s="55">
         <v>17581458.260899998</v>
       </c>
-      <c r="D39" s="68">
-        <f>(C$43-C39)</f>
+      <c r="D39" s="57">
+        <f t="shared" si="0"/>
         <v>-245626.58609999716</v>
       </c>
-      <c r="E39" s="66">
+      <c r="E39" s="55">
         <v>807</v>
       </c>
-      <c r="F39" s="66">
+      <c r="F39" s="55">
         <v>8440</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="67"/>
-      <c r="B40" s="64" t="s">
+      <c r="A40" s="56"/>
+      <c r="B40" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="66">
+      <c r="C40" s="55">
         <v>17575239.285700001</v>
       </c>
-      <c r="D40" s="68">
-        <f>(C$43-C40)</f>
+      <c r="D40" s="57">
+        <f t="shared" si="0"/>
         <v>-239407.61089999974</v>
       </c>
-      <c r="E40" s="66">
+      <c r="E40" s="55">
         <v>475</v>
       </c>
-      <c r="F40" s="66">
+      <c r="F40" s="55">
         <v>5120</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="67"/>
-      <c r="B41" s="64" t="s">
+      <c r="A41" s="56"/>
+      <c r="B41" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="66">
+      <c r="C41" s="55">
         <v>17415497.881900001</v>
       </c>
-      <c r="D41" s="68">
-        <f>(C$43-C41)</f>
+      <c r="D41" s="57">
+        <f t="shared" si="0"/>
         <v>-79666.207100000232</v>
       </c>
-      <c r="E41" s="66">
+      <c r="E41" s="55">
         <v>1018</v>
       </c>
-      <c r="F41" s="66">
+      <c r="F41" s="55">
         <v>10550</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="67"/>
-      <c r="B42" s="64" t="s">
+      <c r="A42" s="56"/>
+      <c r="B42" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="68">
+      <c r="C42" s="57">
         <v>17338096.295000002</v>
       </c>
-      <c r="D42" s="68">
-        <f>(C$43-C42)</f>
+      <c r="D42" s="57">
+        <f t="shared" si="0"/>
         <v>-2264.6202000007033</v>
       </c>
-      <c r="E42" s="66">
+      <c r="E42" s="55">
         <v>948</v>
       </c>
-      <c r="F42" s="66">
+      <c r="F42" s="55">
         <v>9850</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="64"/>
-      <c r="B43" s="64" t="s">
+      <c r="A43" s="53"/>
+      <c r="B43" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="66">
+      <c r="C43" s="55">
         <v>17335831.674800001</v>
       </c>
-      <c r="D43" s="69">
-        <f>(C$43-C43)</f>
+      <c r="D43" s="58">
         <v>0</v>
       </c>
-      <c r="E43" s="66">
+      <c r="E43" s="55">
         <v>948</v>
       </c>
-      <c r="F43" s="66">
+      <c r="F43" s="55">
         <v>9850</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="64" t="s">
+      <c r="A44" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="64" t="s">
+      <c r="B44" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
+      <c r="C44" s="55">
+        <v>20339794.0145</v>
+      </c>
+      <c r="D44" s="57">
+        <f>(C$50-C44)</f>
+        <v>-625450.59039999917</v>
+      </c>
+      <c r="E44" s="55">
+        <v>1</v>
+      </c>
+      <c r="F44" s="55">
+        <v>106</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
+      <c r="C45" s="42">
+        <v>20234313.611400001</v>
+      </c>
+      <c r="D45" s="57">
+        <f t="shared" ref="D45:D50" si="1">(C$50-C45)</f>
+        <v>-519970.18730000034</v>
+      </c>
+      <c r="E45" s="42">
+        <v>178</v>
+      </c>
+      <c r="F45" s="42">
+        <v>1876</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
+      <c r="C46" s="42">
+        <v>20173075.5416</v>
+      </c>
+      <c r="D46" s="57">
+        <f t="shared" si="1"/>
+        <v>-458732.1174999997</v>
+      </c>
+      <c r="E46" s="42">
+        <v>2098</v>
+      </c>
+      <c r="F46" s="42">
+        <v>21076</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
+      <c r="C47" s="42">
+        <v>20161619.082699999</v>
+      </c>
+      <c r="D47" s="57">
+        <f t="shared" si="1"/>
+        <v>-447275.6585999988</v>
+      </c>
+      <c r="E47" s="42">
+        <v>806</v>
+      </c>
+      <c r="F47" s="42">
+        <v>8156</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
+      <c r="C48" s="42">
+        <v>19835805.738699999</v>
+      </c>
+      <c r="D48" s="57">
+        <f t="shared" si="1"/>
+        <v>-121462.3145999983</v>
+      </c>
+      <c r="E48" s="42">
+        <v>1141</v>
+      </c>
+      <c r="F48" s="42">
+        <v>11506</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
+      <c r="C49" s="42">
+        <v>19766846.339600001</v>
+      </c>
+      <c r="D49" s="57">
+        <f t="shared" si="1"/>
+        <v>-52502.915500000119</v>
+      </c>
+      <c r="E49" s="42">
+        <v>1138</v>
+      </c>
+      <c r="F49" s="42">
+        <v>11476</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44"/>
       <c r="B50" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
+      <c r="C50" s="45">
+        <v>19714343.4241</v>
+      </c>
+      <c r="D50" s="77">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="46">
+        <v>1125</v>
+      </c>
+      <c r="F50" s="46">
+        <v>11346</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2819,7 +2884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A140" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
@@ -4717,34 +4782,34 @@
       </c>
     </row>
     <row r="126" spans="1:5" s="6" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="70"/>
-      <c r="B126" s="71">
+      <c r="A126" s="59"/>
+      <c r="B126" s="60">
         <v>24</v>
       </c>
-      <c r="C126" s="72">
+      <c r="C126" s="61">
         <v>5917744.8439999996</v>
       </c>
-      <c r="D126" s="71">
+      <c r="D126" s="60">
         <v>443</v>
       </c>
-      <c r="E126" s="71">
+      <c r="E126" s="60">
         <v>4638</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="73" t="s">
+      <c r="A127" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B127" s="71">
+      <c r="B127" s="60">
         <v>0</v>
       </c>
-      <c r="C127" s="72">
+      <c r="C127" s="61">
         <v>17568788.433699999</v>
       </c>
-      <c r="D127" s="76">
+      <c r="D127" s="63">
         <v>695</v>
       </c>
-      <c r="E127" s="76">
+      <c r="E127" s="63">
         <v>7320</v>
       </c>
     </row>
@@ -4753,13 +4818,13 @@
       <c r="B128" s="4">
         <v>1</v>
       </c>
-      <c r="C128" s="72">
+      <c r="C128" s="61">
         <v>17568345.515299998</v>
       </c>
-      <c r="D128" s="76">
+      <c r="D128" s="63">
         <v>710</v>
       </c>
-      <c r="E128" s="76">
+      <c r="E128" s="63">
         <v>7470</v>
       </c>
     </row>
@@ -4768,13 +4833,13 @@
       <c r="B129" s="4">
         <v>2</v>
       </c>
-      <c r="C129" s="72">
+      <c r="C129" s="61">
         <v>17567925.9791</v>
       </c>
-      <c r="D129" s="76">
+      <c r="D129" s="63">
         <v>709</v>
       </c>
-      <c r="E129" s="76">
+      <c r="E129" s="63">
         <v>7460</v>
       </c>
     </row>
@@ -4783,13 +4848,13 @@
       <c r="B130" s="4">
         <v>3</v>
       </c>
-      <c r="C130" s="72">
+      <c r="C130" s="61">
         <v>17568979.975200001</v>
       </c>
-      <c r="D130" s="76">
+      <c r="D130" s="63">
         <v>708</v>
       </c>
-      <c r="E130" s="76">
+      <c r="E130" s="63">
         <v>7450</v>
       </c>
     </row>
@@ -4798,13 +4863,13 @@
       <c r="B131" s="4">
         <v>4</v>
       </c>
-      <c r="C131" s="72">
+      <c r="C131" s="61">
         <v>17568105.775400002</v>
       </c>
-      <c r="D131" s="76">
+      <c r="D131" s="63">
         <v>723</v>
       </c>
-      <c r="E131" s="76">
+      <c r="E131" s="63">
         <v>7600</v>
       </c>
     </row>
@@ -4813,13 +4878,13 @@
       <c r="B132" s="4">
         <v>5</v>
       </c>
-      <c r="C132" s="72">
+      <c r="C132" s="61">
         <v>17567265.842700001</v>
       </c>
-      <c r="D132" s="76">
+      <c r="D132" s="63">
         <v>736</v>
       </c>
-      <c r="E132" s="76">
+      <c r="E132" s="63">
         <v>7730</v>
       </c>
     </row>
@@ -4828,13 +4893,13 @@
       <c r="B133" s="4">
         <v>6</v>
       </c>
-      <c r="C133" s="72">
+      <c r="C133" s="61">
         <v>17569197.895300001</v>
       </c>
-      <c r="D133" s="76">
+      <c r="D133" s="63">
         <v>700</v>
       </c>
-      <c r="E133" s="76">
+      <c r="E133" s="63">
         <v>7370</v>
       </c>
     </row>
@@ -4843,13 +4908,13 @@
       <c r="B134" s="4">
         <v>7</v>
       </c>
-      <c r="C134" s="72">
+      <c r="C134" s="61">
         <v>17568264.252900001</v>
       </c>
-      <c r="D134" s="76">
+      <c r="D134" s="63">
         <v>678</v>
       </c>
-      <c r="E134" s="76">
+      <c r="E134" s="63">
         <v>7150</v>
       </c>
     </row>
@@ -4858,13 +4923,13 @@
       <c r="B135" s="4">
         <v>8</v>
       </c>
-      <c r="C135" s="72">
+      <c r="C135" s="61">
         <v>17568470.5645</v>
       </c>
-      <c r="D135" s="76">
+      <c r="D135" s="63">
         <v>701</v>
       </c>
-      <c r="E135" s="76">
+      <c r="E135" s="63">
         <v>7380</v>
       </c>
     </row>
@@ -4873,13 +4938,13 @@
       <c r="B136" s="4">
         <v>9</v>
       </c>
-      <c r="C136" s="72">
+      <c r="C136" s="61">
         <v>17567358.417399999</v>
       </c>
-      <c r="D136" s="76">
+      <c r="D136" s="63">
         <v>744</v>
       </c>
-      <c r="E136" s="76">
+      <c r="E136" s="63">
         <v>7810</v>
       </c>
     </row>
@@ -4888,13 +4953,13 @@
       <c r="B137" s="4">
         <v>10</v>
       </c>
-      <c r="C137" s="72">
+      <c r="C137" s="61">
         <v>17567910.4683</v>
       </c>
-      <c r="D137" s="76">
+      <c r="D137" s="63">
         <v>714</v>
       </c>
-      <c r="E137" s="76">
+      <c r="E137" s="63">
         <v>7510</v>
       </c>
     </row>
@@ -4903,13 +4968,13 @@
       <c r="B138" s="4">
         <v>11</v>
       </c>
-      <c r="C138" s="72">
+      <c r="C138" s="61">
         <v>17567562.846000001</v>
       </c>
-      <c r="D138" s="76">
+      <c r="D138" s="63">
         <v>726</v>
       </c>
-      <c r="E138" s="76">
+      <c r="E138" s="63">
         <v>7630</v>
       </c>
     </row>
@@ -4918,13 +4983,13 @@
       <c r="B139" s="4">
         <v>12</v>
       </c>
-      <c r="C139" s="72">
+      <c r="C139" s="61">
         <v>17568503.699999999</v>
       </c>
-      <c r="D139" s="76">
+      <c r="D139" s="63">
         <v>726</v>
       </c>
-      <c r="E139" s="76">
+      <c r="E139" s="63">
         <v>7630</v>
       </c>
     </row>
@@ -4933,13 +4998,13 @@
       <c r="B140" s="4">
         <v>13</v>
       </c>
-      <c r="C140" s="72">
+      <c r="C140" s="61">
         <v>17568406.681699999</v>
       </c>
-      <c r="D140" s="76">
+      <c r="D140" s="63">
         <v>716</v>
       </c>
-      <c r="E140" s="76">
+      <c r="E140" s="63">
         <v>7530</v>
       </c>
     </row>
@@ -4948,13 +5013,13 @@
       <c r="B141" s="4">
         <v>14</v>
       </c>
-      <c r="C141" s="72">
+      <c r="C141" s="61">
         <v>17567663.021699999</v>
       </c>
-      <c r="D141" s="76">
+      <c r="D141" s="63">
         <v>703</v>
       </c>
-      <c r="E141" s="76">
+      <c r="E141" s="63">
         <v>7400</v>
       </c>
     </row>
@@ -4963,13 +5028,13 @@
       <c r="B142" s="4">
         <v>15</v>
       </c>
-      <c r="C142" s="72">
+      <c r="C142" s="61">
         <v>17567352.194699999</v>
       </c>
-      <c r="D142" s="76">
+      <c r="D142" s="63">
         <v>742</v>
       </c>
-      <c r="E142" s="76">
+      <c r="E142" s="63">
         <v>7790</v>
       </c>
     </row>
@@ -4978,13 +5043,13 @@
       <c r="B143" s="4">
         <v>16</v>
       </c>
-      <c r="C143" s="72">
+      <c r="C143" s="61">
         <v>17567777.249899998</v>
       </c>
-      <c r="D143" s="76">
+      <c r="D143" s="63">
         <v>729</v>
       </c>
-      <c r="E143" s="76">
+      <c r="E143" s="63">
         <v>7660</v>
       </c>
     </row>
@@ -4993,13 +5058,13 @@
       <c r="B144" s="4">
         <v>17</v>
       </c>
-      <c r="C144" s="72">
+      <c r="C144" s="61">
         <v>17568344.159899998</v>
       </c>
-      <c r="D144" s="76">
+      <c r="D144" s="63">
         <v>756</v>
       </c>
-      <c r="E144" s="76">
+      <c r="E144" s="63">
         <v>7930</v>
       </c>
     </row>
@@ -5008,13 +5073,13 @@
       <c r="B145" s="4">
         <v>18</v>
       </c>
-      <c r="C145" s="72">
+      <c r="C145" s="61">
         <v>17568257.8365</v>
       </c>
-      <c r="D145" s="76">
+      <c r="D145" s="63">
         <v>734</v>
       </c>
-      <c r="E145" s="76">
+      <c r="E145" s="63">
         <v>7710</v>
       </c>
     </row>
@@ -5023,13 +5088,13 @@
       <c r="B146" s="4">
         <v>19</v>
       </c>
-      <c r="C146" s="72">
+      <c r="C146" s="61">
         <v>17568103.004700001</v>
       </c>
-      <c r="D146" s="76">
+      <c r="D146" s="63">
         <v>712</v>
       </c>
-      <c r="E146" s="76">
+      <c r="E146" s="63">
         <v>7490</v>
       </c>
     </row>
@@ -5038,13 +5103,13 @@
       <c r="B147" s="4">
         <v>20</v>
       </c>
-      <c r="C147" s="72">
+      <c r="C147" s="61">
         <v>17567823.369100001</v>
       </c>
-      <c r="D147" s="76">
+      <c r="D147" s="63">
         <v>706</v>
       </c>
-      <c r="E147" s="76">
+      <c r="E147" s="63">
         <v>7430</v>
       </c>
     </row>
@@ -5053,13 +5118,13 @@
       <c r="B148" s="4">
         <v>21</v>
       </c>
-      <c r="C148" s="72">
+      <c r="C148" s="61">
         <v>17568645.069400001</v>
       </c>
-      <c r="D148" s="76">
+      <c r="D148" s="63">
         <v>733</v>
       </c>
-      <c r="E148" s="76">
+      <c r="E148" s="63">
         <v>7700</v>
       </c>
     </row>
@@ -5068,13 +5133,13 @@
       <c r="B149" s="4">
         <v>22</v>
       </c>
-      <c r="C149" s="72">
+      <c r="C149" s="61">
         <v>17568881.984000001</v>
       </c>
-      <c r="D149" s="76">
+      <c r="D149" s="63">
         <v>688</v>
       </c>
-      <c r="E149" s="76">
+      <c r="E149" s="63">
         <v>7250</v>
       </c>
     </row>
@@ -5083,36 +5148,36 @@
       <c r="B150" s="4">
         <v>23</v>
       </c>
-      <c r="C150" s="72">
+      <c r="C150" s="61">
         <v>17568584.1358</v>
       </c>
-      <c r="D150" s="76">
+      <c r="D150" s="63">
         <v>725</v>
       </c>
-      <c r="E150" s="76">
+      <c r="E150" s="63">
         <v>7620</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="70"/>
-      <c r="B151" s="71">
+      <c r="A151" s="59"/>
+      <c r="B151" s="60">
         <v>24</v>
       </c>
-      <c r="C151" s="72">
+      <c r="C151" s="61">
         <v>17568345.150800001</v>
       </c>
-      <c r="D151" s="76">
+      <c r="D151" s="63">
         <v>708</v>
       </c>
-      <c r="E151" s="76">
+      <c r="E151" s="63">
         <v>7450</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="73" t="s">
+      <c r="A152" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="B152" s="71">
+      <c r="B152" s="60">
         <v>0</v>
       </c>
     </row>
@@ -5232,7 +5297,7 @@
       </c>
     </row>
     <row r="176" spans="2:2" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B176" s="71">
+      <c r="B176" s="60">
         <v>24</v>
       </c>
     </row>
@@ -5258,8 +5323,8 @@
   <sheetData>
     <row r="1" spans="1:12" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
       <c r="D1" s="28" t="s">
         <v>26</v>
       </c>
@@ -5287,38 +5352,38 @@
       <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" s="26" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="61"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="73"/>
     </row>
     <row r="3" spans="1:12" s="26" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="56"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="72"/>
     </row>
     <row r="4" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="29" t="s">
         <v>40</v>
       </c>
@@ -5349,8 +5414,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="29" t="s">
         <v>41</v>
       </c>
@@ -5381,8 +5446,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="29" t="s">
         <v>42</v>
       </c>
@@ -5413,38 +5478,38 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="26" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="56"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="72"/>
     </row>
     <row r="8" spans="1:12" s="26" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="56"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="72"/>
     </row>
     <row r="9" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="56"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="29" t="s">
         <v>40</v>
       </c>
@@ -5475,8 +5540,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="56"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="29" t="s">
         <v>41</v>
       </c>
@@ -5507,8 +5572,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="29" t="s">
         <v>42</v>
       </c>
@@ -5539,38 +5604,38 @@
       </c>
     </row>
     <row r="12" spans="1:12" s="26" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="56"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="72"/>
     </row>
     <row r="13" spans="1:12" s="26" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="56"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="72"/>
     </row>
     <row r="14" spans="1:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="56"/>
-      <c r="B14" s="56"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="29" t="s">
         <v>40</v>
       </c>
@@ -5601,8 +5666,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="56"/>
-      <c r="B15" s="56"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="29" t="s">
         <v>41</v>
       </c>
@@ -5633,8 +5698,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
+      <c r="A16" s="76"/>
+      <c r="B16" s="76"/>
       <c r="C16" s="31" t="s">
         <v>42</v>
       </c>
@@ -5669,16 +5734,21 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="K2:K3"/>
@@ -5694,21 +5764,16 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated Tables and Figs
added results of Prebus and Branstetter
</commit_message>
<xml_diff>
--- a/Tables-Figures/Tables/Tables.xlsx
+++ b/Tables-Figures/Tables/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="460" windowWidth="20360" windowHeight="14760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="5240" yWindow="460" windowWidth="20360" windowHeight="14700" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tab1-datasets" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="69">
   <si>
     <t>AICc</t>
   </si>
@@ -122,15 +122,6 @@
   </si>
   <si>
     <t>Moyle</t>
-  </si>
-  <si>
-    <t>0verall</t>
-  </si>
-  <si>
-    <t>EN (means)</t>
-  </si>
-  <si>
-    <t>GC (means)</t>
   </si>
   <si>
     <t>Datasets</t>
@@ -249,6 +240,12 @@
   </si>
   <si>
     <t>Prebus et al. 2017</t>
+  </si>
+  <si>
+    <t>UCE dataset</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
 </sst>
 </file>
@@ -271,13 +268,11 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <u/>
@@ -300,26 +295,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="9"/>
@@ -332,7 +323,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="11"/>
@@ -351,13 +341,11 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="161"/>
     </font>
   </fonts>
   <fills count="2">
@@ -435,7 +423,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -453,8 +441,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -554,6 +554,90 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -563,128 +647,49 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -693,6 +698,12 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -701,6 +712,12 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -979,20 +996,20 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="6" width="11.83203125" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" style="39" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>9</v>
@@ -1015,50 +1032,50 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="10">
-        <v>465241</v>
-      </c>
-      <c r="E2" s="10">
-        <v>1143</v>
-      </c>
-      <c r="F2" s="10">
-        <v>10</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>3</v>
+      <c r="A2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="49">
+        <v>183747</v>
+      </c>
+      <c r="E2" s="49">
+        <v>807</v>
+      </c>
+      <c r="F2" s="49">
+        <v>187</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>59</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="10">
-        <v>539526</v>
+        <v>465241</v>
       </c>
       <c r="E3" s="10">
-        <v>1537</v>
+        <v>1143</v>
       </c>
       <c r="F3" s="10">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1088,97 +1105,97 @@
     </row>
     <row r="5" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10">
+        <v>539526</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1537</v>
+      </c>
+      <c r="F5" s="10">
+        <v>33</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="10">
         <v>599627</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E6" s="10">
         <v>1479</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F6" s="10">
         <v>18</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="52">
-        <v>375172</v>
-      </c>
-      <c r="E6" s="52">
-        <v>515</v>
-      </c>
-      <c r="F6" s="52">
-        <v>106</v>
-      </c>
-      <c r="G6" s="52" t="s">
-        <v>7</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="52">
-        <v>183747</v>
-      </c>
-      <c r="E7" s="52">
-        <v>807</v>
-      </c>
-      <c r="F7" s="52">
-        <v>187</v>
-      </c>
-      <c r="G7" s="52" t="s">
-        <v>62</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="49">
+        <v>375172</v>
+      </c>
+      <c r="E7" s="49">
+        <v>515</v>
+      </c>
+      <c r="F7" s="49">
+        <v>106</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>7</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="47">
+        <v>1561581</v>
+      </c>
+      <c r="E8" s="47">
+        <v>2098</v>
+      </c>
+      <c r="F8" s="47">
+        <v>50</v>
+      </c>
+      <c r="G8" s="47" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="49">
-        <v>1561581</v>
-      </c>
-      <c r="E8" s="49">
-        <v>2098</v>
-      </c>
-      <c r="F8" s="49">
-        <v>50</v>
-      </c>
-      <c r="G8" s="49" t="s">
-        <v>69</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1191,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1204,50 +1221,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
+      <c r="D1" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>27</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="H2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>63</v>
-      </c>
       <c r="I2" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="64"/>
+      <c r="A3" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="67"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -1259,25 +1275,25 @@
     </row>
     <row r="4" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="12">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="D4" s="12">
         <v>0.21190000000000001</v>
-      </c>
-      <c r="D4" s="12">
-        <v>9.6530000000000005E-2</v>
       </c>
       <c r="E4" s="12">
         <v>0.2782</v>
       </c>
       <c r="F4" s="12">
+        <v>9.6530000000000005E-2</v>
+      </c>
+      <c r="G4" s="12">
         <v>5.475E-2</v>
       </c>
-      <c r="G4" s="12">
+      <c r="H4" s="12">
         <v>0.13969999999999999</v>
-      </c>
-      <c r="H4" s="12">
-        <v>0.82799999999999996</v>
       </c>
       <c r="I4" s="10">
         <v>0.182</v>
@@ -1289,25 +1305,25 @@
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="12">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="D5" s="12">
         <v>7.1760000000000004E-2</v>
-      </c>
-      <c r="D5" s="12">
-        <v>3.0980000000000001E-2</v>
       </c>
       <c r="E5" s="12">
         <v>8.9700000000000002E-2</v>
       </c>
       <c r="F5" s="12">
+        <v>3.0980000000000001E-2</v>
+      </c>
+      <c r="G5" s="12">
         <v>1.5429999999999999E-2</v>
       </c>
-      <c r="G5" s="12">
+      <c r="H5" s="12">
         <v>5.3519999999999998E-2</v>
-      </c>
-      <c r="H5" s="12">
-        <v>0.23599999999999999</v>
       </c>
       <c r="I5" s="12">
         <v>0.122</v>
@@ -1320,39 +1336,39 @@
     <row r="6" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="12">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="D6" s="12">
         <v>0.14510000000000001</v>
-      </c>
-      <c r="D6" s="12">
-        <v>5.8900000000000001E-2</v>
       </c>
       <c r="E6" s="12">
         <v>0.26719999999999999</v>
       </c>
       <c r="F6" s="12">
+        <v>5.8900000000000001E-2</v>
+      </c>
+      <c r="G6" s="12">
         <v>3.5979999999999998E-2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="H6" s="12">
         <v>9.0069999999999997E-2</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0.83099999999999996</v>
       </c>
       <c r="I6" s="12">
         <v>0.18099999999999999</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="0"/>
-        <v>0.22989285714285712</v>
+        <v>0.22989285714285715</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="65"/>
+      <c r="A7" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="68"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -1364,92 +1380,92 @@
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="13">
+        <v>32.909999999999997</v>
+      </c>
+      <c r="D8" s="13">
         <v>31.39</v>
-      </c>
-      <c r="D8" s="13">
-        <v>28.42</v>
       </c>
       <c r="E8" s="13">
         <v>40.119999999999997</v>
       </c>
       <c r="F8" s="13">
+        <v>28.42</v>
+      </c>
+      <c r="G8" s="13">
         <v>36.1</v>
       </c>
-      <c r="G8" s="13">
+      <c r="H8" s="13">
         <v>33.61</v>
-      </c>
-      <c r="H8" s="13">
-        <v>32.909999999999997</v>
       </c>
       <c r="I8" s="13">
         <v>36.58</v>
       </c>
       <c r="J8" s="13">
         <f>AVERAGE(C8:I8)</f>
-        <v>34.161428571428573</v>
+        <v>34.161428571428566</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="10">
+        <v>38</v>
+      </c>
+      <c r="C9" s="13">
+        <v>43.1</v>
+      </c>
+      <c r="D9" s="10">
         <v>41.02</v>
-      </c>
-      <c r="D9" s="10">
-        <v>34.090000000000003</v>
       </c>
       <c r="E9" s="10">
         <v>46.68</v>
       </c>
       <c r="F9" s="10">
+        <v>34.090000000000003</v>
+      </c>
+      <c r="G9" s="10">
         <v>43.38</v>
       </c>
-      <c r="G9" s="10">
+      <c r="H9" s="10">
         <v>44.38</v>
-      </c>
-      <c r="H9" s="13">
-        <v>43.1</v>
       </c>
       <c r="I9" s="10">
         <v>48.04</v>
       </c>
       <c r="J9" s="13">
-        <f t="shared" ref="J9:J10" si="1">AVERAGE(C9:I9)</f>
+        <f>AVERAGE(C9:I9)</f>
         <v>42.955714285714286</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="9" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="14">
+        <v>39</v>
+      </c>
+      <c r="C10" s="47">
+        <v>32.24</v>
+      </c>
+      <c r="D10" s="14">
         <v>30.99</v>
-      </c>
-      <c r="D10" s="23">
-        <v>28.75</v>
       </c>
       <c r="E10" s="23">
         <v>40.47</v>
       </c>
       <c r="F10" s="23">
+        <v>28.75</v>
+      </c>
+      <c r="G10" s="23">
         <v>36.61</v>
       </c>
-      <c r="G10" s="23">
+      <c r="H10" s="23">
         <v>33.5</v>
       </c>
-      <c r="H10" s="49">
-        <v>32.24</v>
-      </c>
-      <c r="I10" s="49">
+      <c r="I10" s="47">
         <v>36.94</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(C10:I10)</f>
         <v>34.214285714285715</v>
       </c>
     </row>
@@ -1457,7 +1473,7 @@
   <mergeCells count="3">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="D1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1467,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,931 +1493,931 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="52">
+        <v>17672425.579100002</v>
+      </c>
+      <c r="D2" s="54">
+        <f t="shared" ref="D2:D7" si="0">(C$8-C2)</f>
+        <v>-336593.90430000052</v>
+      </c>
+      <c r="E2" s="52">
+        <v>1</v>
+      </c>
+      <c r="F2" s="52">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="53"/>
+      <c r="B3" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="52">
+        <v>17591017.273499999</v>
+      </c>
+      <c r="D3" s="54">
+        <f t="shared" si="0"/>
+        <v>-255185.59869999811</v>
+      </c>
+      <c r="E3" s="52">
+        <v>158</v>
+      </c>
+      <c r="F3" s="52">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="53"/>
+      <c r="B4" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="52">
+        <v>17581458.260899998</v>
+      </c>
+      <c r="D4" s="54">
+        <f t="shared" si="0"/>
+        <v>-245626.58609999716</v>
+      </c>
+      <c r="E4" s="52">
+        <v>807</v>
+      </c>
+      <c r="F4" s="52">
+        <v>8440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="53"/>
+      <c r="B5" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="52">
+        <v>17575239.285700001</v>
+      </c>
+      <c r="D5" s="54">
+        <f t="shared" si="0"/>
+        <v>-239407.61089999974</v>
+      </c>
+      <c r="E5" s="52">
+        <v>475</v>
+      </c>
+      <c r="F5" s="52">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="53"/>
+      <c r="B6" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="52">
+        <v>17415497.881900001</v>
+      </c>
+      <c r="D6" s="54">
+        <f t="shared" si="0"/>
+        <v>-79666.207100000232</v>
+      </c>
+      <c r="E6" s="52">
+        <v>1018</v>
+      </c>
+      <c r="F6" s="52">
+        <v>10550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="53"/>
+      <c r="B7" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="54">
+        <v>17338096.295000002</v>
+      </c>
+      <c r="D7" s="54">
+        <f t="shared" si="0"/>
+        <v>-2264.6202000007033</v>
+      </c>
+      <c r="E7" s="52">
+        <v>948</v>
+      </c>
+      <c r="F7" s="52">
+        <v>9850</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="52">
+        <v>17335831.674800001</v>
+      </c>
+      <c r="D8" s="55">
+        <v>0</v>
+      </c>
+      <c r="E8" s="52">
+        <v>948</v>
+      </c>
+      <c r="F8" s="52">
+        <v>9850</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="40" t="s">
+      <c r="B9" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="40">
+        <v>2481257.25</v>
+      </c>
+      <c r="D9" s="40">
+        <v>-100298.83</v>
+      </c>
+      <c r="E9" s="40">
         <v>1</v>
       </c>
-      <c r="F1" s="40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="42">
-        <v>2481257.25</v>
-      </c>
-      <c r="D2" s="42">
-        <v>-100298.83</v>
-      </c>
-      <c r="E2" s="42">
-        <v>1</v>
-      </c>
-      <c r="F2" s="42">
+      <c r="F9" s="40">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="42">
-        <v>2458688.9500000002</v>
-      </c>
-      <c r="D3" s="42">
-        <v>-77730.53</v>
-      </c>
-      <c r="E3" s="42">
-        <v>85</v>
-      </c>
-      <c r="F3" s="42">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="42">
-        <v>2467719.0299999998</v>
-      </c>
-      <c r="D4" s="42">
-        <v>-86760.61</v>
-      </c>
-      <c r="E4" s="42">
-        <v>1145</v>
-      </c>
-      <c r="F4" s="42">
-        <v>11466</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="42">
-        <v>2456062.62</v>
-      </c>
-      <c r="D5" s="42">
-        <v>-75104.2</v>
-      </c>
-      <c r="E5" s="42">
-        <v>222</v>
-      </c>
-      <c r="F5" s="42">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="42">
-        <v>2410728.44</v>
-      </c>
-      <c r="D6" s="42">
-        <v>-29770.02</v>
-      </c>
-      <c r="E6" s="42">
-        <v>456</v>
-      </c>
-      <c r="F6" s="42">
-        <v>4576</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="42">
-        <v>2397171.3199999998</v>
-      </c>
-      <c r="D7" s="42">
-        <v>-16212.9</v>
-      </c>
-      <c r="E7" s="42">
-        <v>461</v>
-      </c>
-      <c r="F7" s="42">
-        <v>4626</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="43">
-        <v>2380958.42</v>
-      </c>
-      <c r="D8" s="43">
-        <v>0</v>
-      </c>
-      <c r="E8" s="42">
-        <v>452</v>
-      </c>
-      <c r="F8" s="42">
-        <v>4536</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="42">
-        <v>3192533.02</v>
-      </c>
-      <c r="D9" s="42">
-        <v>-137222.82999999999</v>
-      </c>
-      <c r="E9" s="42">
-        <v>1</v>
-      </c>
-      <c r="F9" s="42">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
-      <c r="B10" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="42">
-        <v>3166285.99</v>
-      </c>
-      <c r="D10" s="42">
-        <v>-110975.8</v>
-      </c>
-      <c r="E10" s="42">
-        <v>101</v>
-      </c>
-      <c r="F10" s="42">
-        <v>1072</v>
+      <c r="B10" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="40">
+        <v>2458688.9500000002</v>
+      </c>
+      <c r="D10" s="40">
+        <v>-77730.53</v>
+      </c>
+      <c r="E10" s="40">
+        <v>85</v>
+      </c>
+      <c r="F10" s="40">
+        <v>866</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
-      <c r="B11" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="42">
-        <v>3162976.03</v>
-      </c>
-      <c r="D11" s="42">
-        <v>-107665.84</v>
-      </c>
-      <c r="E11" s="42">
-        <v>1541</v>
-      </c>
-      <c r="F11" s="42">
-        <v>15472</v>
+      <c r="B11" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="40">
+        <v>2467719.0299999998</v>
+      </c>
+      <c r="D11" s="40">
+        <v>-86760.61</v>
+      </c>
+      <c r="E11" s="40">
+        <v>1145</v>
+      </c>
+      <c r="F11" s="40">
+        <v>11466</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
-      <c r="B12" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="42">
-        <v>3147457.96</v>
-      </c>
-      <c r="D12" s="42">
-        <v>-92147.77</v>
-      </c>
-      <c r="E12" s="42">
-        <v>318</v>
-      </c>
-      <c r="F12" s="42">
-        <v>3242</v>
+      <c r="B12" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="40">
+        <v>2456062.62</v>
+      </c>
+      <c r="D12" s="40">
+        <v>-75104.2</v>
+      </c>
+      <c r="E12" s="40">
+        <v>222</v>
+      </c>
+      <c r="F12" s="40">
+        <v>2236</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
-      <c r="B13" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="42">
-        <v>3088673.34</v>
-      </c>
-      <c r="D13" s="42">
-        <v>-33363.15</v>
-      </c>
-      <c r="E13" s="42">
-        <v>615</v>
-      </c>
-      <c r="F13" s="42">
-        <v>6212</v>
+      <c r="B13" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="40">
+        <v>2410728.44</v>
+      </c>
+      <c r="D13" s="40">
+        <v>-29770.02</v>
+      </c>
+      <c r="E13" s="40">
+        <v>456</v>
+      </c>
+      <c r="F13" s="40">
+        <v>4576</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
-      <c r="B14" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="42">
-        <v>3094082.23</v>
-      </c>
-      <c r="D14" s="42">
-        <v>-38772.04</v>
-      </c>
-      <c r="E14" s="42">
-        <v>638</v>
-      </c>
-      <c r="F14" s="42">
-        <v>6442</v>
+      <c r="B14" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="40">
+        <v>2397171.3199999998</v>
+      </c>
+      <c r="D14" s="40">
+        <v>-16212.9</v>
+      </c>
+      <c r="E14" s="40">
+        <v>461</v>
+      </c>
+      <c r="F14" s="40">
+        <v>4626</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
-      <c r="B15" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="43">
-        <v>3055310.19</v>
-      </c>
-      <c r="D15" s="43">
+      <c r="B15" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="41">
+        <v>2380958.42</v>
+      </c>
+      <c r="D15" s="41">
         <v>0</v>
       </c>
-      <c r="E15" s="42">
-        <v>586</v>
-      </c>
-      <c r="F15" s="42">
-        <v>5922</v>
+      <c r="E15" s="40">
+        <v>452</v>
+      </c>
+      <c r="F15" s="40">
+        <v>4536</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="42">
+      <c r="B16" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="40">
         <v>3833182.37</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="40">
         <v>-145227.91</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="40">
         <v>1</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="40">
         <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
-      <c r="B17" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="42">
+      <c r="B17" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="40">
         <v>3800797.49</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="40">
         <v>-112843.03</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="40">
         <v>114</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="40">
         <v>1246</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
-      <c r="B18" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="42">
+      <c r="B18" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="40">
         <v>3796629.28</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="40">
         <v>-108674.82</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="40">
         <v>596</v>
       </c>
-      <c r="F18" s="42">
+      <c r="F18" s="40">
         <v>6066</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
-      <c r="B19" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="42">
+      <c r="B19" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="40">
         <v>3793471.49</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="40">
         <v>-105517.03</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="40">
         <v>267</v>
       </c>
-      <c r="F19" s="42">
+      <c r="F19" s="40">
         <v>2776</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
-      <c r="B20" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="42">
+      <c r="B20" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="40">
         <v>3736560.33</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="40">
         <v>-48605.87</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="40">
         <v>513</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="40">
         <v>5236</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="42">
+      <c r="B21" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="40">
         <v>3695066.87</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="40">
         <v>-7112.41</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="40">
         <v>493</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F21" s="40">
         <v>5036</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-      <c r="B22" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="43">
+      <c r="B22" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="41">
         <v>3687954.46</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="41">
         <v>0</v>
       </c>
-      <c r="E22" s="42">
+      <c r="E22" s="40">
         <v>493</v>
       </c>
-      <c r="F22" s="42">
+      <c r="F22" s="40">
         <v>5036</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="42">
-        <v>2339168.0099999998</v>
-      </c>
-      <c r="D23" s="42">
-        <v>-100584.4</v>
-      </c>
-      <c r="E23" s="42">
+      <c r="A23" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="40">
+        <v>3192533.02</v>
+      </c>
+      <c r="D23" s="40">
+        <v>-137222.82999999999</v>
+      </c>
+      <c r="E23" s="40">
         <v>1</v>
       </c>
-      <c r="F23" s="42">
-        <v>42</v>
+      <c r="F23" s="40">
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
-      <c r="B24" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="42">
-        <v>2314873.86</v>
-      </c>
-      <c r="D24" s="42">
-        <v>-76290.25</v>
-      </c>
-      <c r="E24" s="42">
-        <v>97</v>
-      </c>
-      <c r="F24" s="42">
-        <v>1002</v>
+      <c r="B24" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="40">
+        <v>3166285.99</v>
+      </c>
+      <c r="D24" s="40">
+        <v>-110975.8</v>
+      </c>
+      <c r="E24" s="40">
+        <v>101</v>
+      </c>
+      <c r="F24" s="40">
+        <v>1072</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
-      <c r="B25" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="42">
-        <v>2316403.81</v>
-      </c>
-      <c r="D25" s="42">
-        <v>-77820.2</v>
-      </c>
-      <c r="E25" s="42">
-        <v>1479</v>
-      </c>
-      <c r="F25" s="42">
-        <v>14822</v>
+      <c r="B25" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="40">
+        <v>3162976.03</v>
+      </c>
+      <c r="D25" s="40">
+        <v>-107665.84</v>
+      </c>
+      <c r="E25" s="40">
+        <v>1541</v>
+      </c>
+      <c r="F25" s="40">
+        <v>15472</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
-      <c r="B26" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="42">
-        <v>2299674.11</v>
-      </c>
-      <c r="D26" s="42">
-        <v>-61090.5</v>
-      </c>
-      <c r="E26" s="42">
-        <v>249</v>
-      </c>
-      <c r="F26" s="42">
-        <v>2522</v>
+      <c r="B26" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="40">
+        <v>3147457.96</v>
+      </c>
+      <c r="D26" s="40">
+        <v>-92147.77</v>
+      </c>
+      <c r="E26" s="40">
+        <v>318</v>
+      </c>
+      <c r="F26" s="40">
+        <v>3242</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-      <c r="B27" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="42">
-        <v>2255397.7200000002</v>
-      </c>
-      <c r="D27" s="42">
-        <v>-16814.11</v>
-      </c>
-      <c r="E27" s="42">
-        <v>463</v>
-      </c>
-      <c r="F27" s="42">
-        <v>4662</v>
+      <c r="B27" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="40">
+        <v>3088673.34</v>
+      </c>
+      <c r="D27" s="40">
+        <v>-33363.15</v>
+      </c>
+      <c r="E27" s="40">
+        <v>615</v>
+      </c>
+      <c r="F27" s="40">
+        <v>6212</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
-      <c r="B28" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="42">
-        <v>2254128.23</v>
-      </c>
-      <c r="D28" s="42">
-        <v>-15544.62</v>
-      </c>
-      <c r="E28" s="42">
-        <v>471</v>
-      </c>
-      <c r="F28" s="42">
-        <v>4742</v>
+      <c r="B28" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="40">
+        <v>3094082.23</v>
+      </c>
+      <c r="D28" s="40">
+        <v>-38772.04</v>
+      </c>
+      <c r="E28" s="40">
+        <v>638</v>
+      </c>
+      <c r="F28" s="40">
+        <v>6442</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
-      <c r="B29" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="43">
-        <v>2238583.61</v>
-      </c>
-      <c r="D29" s="43">
+      <c r="B29" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="41">
+        <v>3055310.19</v>
+      </c>
+      <c r="D29" s="41">
         <v>0</v>
       </c>
-      <c r="E29" s="42">
-        <v>458</v>
-      </c>
-      <c r="F29" s="42">
-        <v>4612</v>
+      <c r="E29" s="40">
+        <v>586</v>
+      </c>
+      <c r="F29" s="40">
+        <v>5922</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="42">
-        <v>6005671.7599999998</v>
-      </c>
-      <c r="D30" s="42">
-        <v>-230918.31</v>
-      </c>
-      <c r="E30" s="42">
+      <c r="A30" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="40">
+        <v>2339168.0099999998</v>
+      </c>
+      <c r="D30" s="40">
+        <v>-100584.4</v>
+      </c>
+      <c r="E30" s="40">
         <v>1</v>
       </c>
-      <c r="F30" s="42">
-        <v>218</v>
+      <c r="F30" s="40">
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
-      <c r="B31" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="42">
-        <v>5936151.6299999999</v>
-      </c>
-      <c r="D31" s="42">
-        <v>-161398.18</v>
-      </c>
-      <c r="E31" s="42">
-        <v>200</v>
-      </c>
-      <c r="F31" s="42">
-        <v>2208</v>
+      <c r="B31" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="40">
+        <v>2314873.86</v>
+      </c>
+      <c r="D31" s="40">
+        <v>-76290.25</v>
+      </c>
+      <c r="E31" s="40">
+        <v>97</v>
+      </c>
+      <c r="F31" s="40">
+        <v>1002</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
-      <c r="B32" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="42">
-        <v>5937376.8200000003</v>
-      </c>
-      <c r="D32" s="42">
-        <v>-162623.37</v>
-      </c>
-      <c r="E32" s="42">
-        <v>515</v>
-      </c>
-      <c r="F32" s="42">
-        <v>5358</v>
+      <c r="B32" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="40">
+        <v>2316403.81</v>
+      </c>
+      <c r="D32" s="40">
+        <v>-77820.2</v>
+      </c>
+      <c r="E32" s="40">
+        <v>1479</v>
+      </c>
+      <c r="F32" s="40">
+        <v>14822</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="B33" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="42">
-        <v>5935114.2599999998</v>
-      </c>
-      <c r="D33" s="42">
-        <v>-160360.81</v>
-      </c>
-      <c r="E33" s="42">
-        <v>271</v>
-      </c>
-      <c r="F33" s="42">
-        <v>2918</v>
+      <c r="B33" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="40">
+        <v>2299674.11</v>
+      </c>
+      <c r="D33" s="40">
+        <v>-61090.5</v>
+      </c>
+      <c r="E33" s="40">
+        <v>249</v>
+      </c>
+      <c r="F33" s="40">
+        <v>2522</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
-      <c r="B34" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="42">
-        <v>5839663.7699999996</v>
-      </c>
-      <c r="D34" s="42">
-        <v>-64910.32</v>
-      </c>
-      <c r="E34" s="42">
-        <v>520</v>
-      </c>
-      <c r="F34" s="42">
-        <v>5408</v>
+      <c r="B34" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="40">
+        <v>2255397.7200000002</v>
+      </c>
+      <c r="D34" s="40">
+        <v>-16814.11</v>
+      </c>
+      <c r="E34" s="40">
+        <v>463</v>
+      </c>
+      <c r="F34" s="40">
+        <v>4662</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
-      <c r="B35" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="42">
+      <c r="B35" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="40">
+        <v>2254128.23</v>
+      </c>
+      <c r="D35" s="40">
+        <v>-15544.62</v>
+      </c>
+      <c r="E35" s="40">
+        <v>471</v>
+      </c>
+      <c r="F35" s="40">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="41">
+        <v>2238583.61</v>
+      </c>
+      <c r="D36" s="41">
+        <v>0</v>
+      </c>
+      <c r="E36" s="40">
+        <v>458</v>
+      </c>
+      <c r="F36" s="40">
+        <v>4612</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="40">
+        <v>6005671.7599999998</v>
+      </c>
+      <c r="D37" s="40">
+        <v>-230918.31</v>
+      </c>
+      <c r="E37" s="40">
+        <v>1</v>
+      </c>
+      <c r="F37" s="40">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="40">
+        <v>5936151.6299999999</v>
+      </c>
+      <c r="D38" s="40">
+        <v>-161398.18</v>
+      </c>
+      <c r="E38" s="40">
+        <v>200</v>
+      </c>
+      <c r="F38" s="40">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="40">
+        <v>5937376.8200000003</v>
+      </c>
+      <c r="D39" s="40">
+        <v>-162623.37</v>
+      </c>
+      <c r="E39" s="40">
+        <v>515</v>
+      </c>
+      <c r="F39" s="40">
+        <v>5358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="40">
+        <v>5935114.2599999998</v>
+      </c>
+      <c r="D40" s="40">
+        <v>-160360.81</v>
+      </c>
+      <c r="E40" s="40">
+        <v>271</v>
+      </c>
+      <c r="F40" s="40">
+        <v>2918</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="40">
+        <v>5839663.7699999996</v>
+      </c>
+      <c r="D41" s="40">
+        <v>-64910.32</v>
+      </c>
+      <c r="E41" s="40">
+        <v>520</v>
+      </c>
+      <c r="F41" s="40">
+        <v>5408</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="40">
         <v>5820918.0899999999</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D42" s="40">
         <v>-46164.639999999999</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E42" s="40">
         <v>496</v>
       </c>
-      <c r="F35" s="42">
+      <c r="F42" s="40">
         <v>5168</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="53"/>
-      <c r="B36" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="54">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="50"/>
+      <c r="B43" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="51">
         <v>5774753.4500000002</v>
       </c>
-      <c r="D36" s="54">
+      <c r="D43" s="51">
         <v>0</v>
       </c>
-      <c r="E36" s="55">
+      <c r="E43" s="52">
         <v>496</v>
       </c>
-      <c r="F36" s="55">
+      <c r="F43" s="52">
         <v>5168</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="55">
-        <v>17672425.579100002</v>
-      </c>
-      <c r="D37" s="57">
-        <f t="shared" ref="D37:D43" si="0">(C$43-C37)</f>
-        <v>-336593.90430000052</v>
-      </c>
-      <c r="E37" s="55">
-        <v>1</v>
-      </c>
-      <c r="F37" s="55">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="56"/>
-      <c r="B38" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="55">
-        <v>17591017.273499999</v>
-      </c>
-      <c r="D38" s="57">
-        <f t="shared" si="0"/>
-        <v>-255185.59869999811</v>
-      </c>
-      <c r="E38" s="55">
-        <v>158</v>
-      </c>
-      <c r="F38" s="55">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="56"/>
-      <c r="B39" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="55">
-        <v>17581458.260899998</v>
-      </c>
-      <c r="D39" s="57">
-        <f t="shared" si="0"/>
-        <v>-245626.58609999716</v>
-      </c>
-      <c r="E39" s="55">
-        <v>807</v>
-      </c>
-      <c r="F39" s="55">
-        <v>8440</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="56"/>
-      <c r="B40" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="55">
-        <v>17575239.285700001</v>
-      </c>
-      <c r="D40" s="57">
-        <f t="shared" si="0"/>
-        <v>-239407.61089999974</v>
-      </c>
-      <c r="E40" s="55">
-        <v>475</v>
-      </c>
-      <c r="F40" s="55">
-        <v>5120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="56"/>
-      <c r="B41" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="55">
-        <v>17415497.881900001</v>
-      </c>
-      <c r="D41" s="57">
-        <f t="shared" si="0"/>
-        <v>-79666.207100000232</v>
-      </c>
-      <c r="E41" s="55">
-        <v>1018</v>
-      </c>
-      <c r="F41" s="55">
-        <v>10550</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="56"/>
-      <c r="B42" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="57">
-        <v>17338096.295000002</v>
-      </c>
-      <c r="D42" s="57">
-        <f t="shared" si="0"/>
-        <v>-2264.6202000007033</v>
-      </c>
-      <c r="E42" s="55">
-        <v>948</v>
-      </c>
-      <c r="F42" s="55">
-        <v>9850</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="53"/>
-      <c r="B43" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="55">
-        <v>17335831.674800001</v>
-      </c>
-      <c r="D43" s="58">
-        <v>0</v>
-      </c>
-      <c r="E43" s="55">
-        <v>948</v>
-      </c>
-      <c r="F43" s="55">
-        <v>9850</v>
-      </c>
-    </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="55">
+      <c r="A44" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="52">
         <v>20339794.0145</v>
       </c>
-      <c r="D44" s="57">
+      <c r="D44" s="54">
         <f>(C$50-C44)</f>
         <v>-625450.59039999917</v>
       </c>
-      <c r="E44" s="55">
+      <c r="E44" s="52">
         <v>1</v>
       </c>
-      <c r="F44" s="55">
+      <c r="F44" s="52">
         <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
-      <c r="B45" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="42">
+      <c r="B45" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="40">
         <v>20234313.611400001</v>
       </c>
-      <c r="D45" s="57">
+      <c r="D45" s="54">
         <f t="shared" ref="D45:D50" si="1">(C$50-C45)</f>
         <v>-519970.18730000034</v>
       </c>
-      <c r="E45" s="42">
+      <c r="E45" s="40">
         <v>178</v>
       </c>
-      <c r="F45" s="42">
+      <c r="F45" s="40">
         <v>1876</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
-      <c r="B46" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="42">
+      <c r="B46" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="40">
         <v>20173075.5416</v>
       </c>
-      <c r="D46" s="57">
+      <c r="D46" s="54">
         <f t="shared" si="1"/>
         <v>-458732.1174999997</v>
       </c>
-      <c r="E46" s="42">
+      <c r="E46" s="40">
         <v>2098</v>
       </c>
-      <c r="F46" s="42">
+      <c r="F46" s="40">
         <v>21076</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="42">
+      <c r="B47" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="40">
         <v>20161619.082699999</v>
       </c>
-      <c r="D47" s="57">
+      <c r="D47" s="54">
         <f t="shared" si="1"/>
         <v>-447275.6585999988</v>
       </c>
-      <c r="E47" s="42">
+      <c r="E47" s="40">
         <v>806</v>
       </c>
-      <c r="F47" s="42">
+      <c r="F47" s="40">
         <v>8156</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="B48" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="42">
+      <c r="B48" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="40">
         <v>19835805.738699999</v>
       </c>
-      <c r="D48" s="57">
+      <c r="D48" s="54">
         <f t="shared" si="1"/>
         <v>-121462.3145999983</v>
       </c>
-      <c r="E48" s="42">
+      <c r="E48" s="40">
         <v>1141</v>
       </c>
-      <c r="F48" s="42">
+      <c r="F48" s="40">
         <v>11506</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
-      <c r="B49" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="42">
+      <c r="B49" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="40">
         <v>19766846.339600001</v>
       </c>
-      <c r="D49" s="57">
+      <c r="D49" s="54">
         <f t="shared" si="1"/>
         <v>-52502.915500000119</v>
       </c>
-      <c r="E49" s="42">
+      <c r="E49" s="40">
         <v>1138</v>
       </c>
-      <c r="F49" s="42">
+      <c r="F49" s="40">
         <v>11476</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="45">
+      <c r="A50" s="42"/>
+      <c r="B50" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="43">
         <v>19714343.4241</v>
       </c>
-      <c r="D50" s="77">
+      <c r="D50" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E50" s="46">
+      <c r="E50" s="44">
         <v>1125</v>
       </c>
-      <c r="F50" s="46">
+      <c r="F50" s="44">
         <v>11346</v>
       </c>
     </row>
@@ -2412,466 +2428,642 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="39" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="38" customWidth="1"/>
-    <col min="3" max="4" width="16.1640625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="36" customWidth="1"/>
+    <col min="3" max="4" width="16.1640625" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>59</v>
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C3" s="63">
+        <v>1.081</v>
+      </c>
+      <c r="D3" s="63">
+        <v>89.465000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="62"/>
+      <c r="B4" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="63">
+        <v>1.038</v>
+      </c>
+      <c r="D4" s="63">
+        <v>514.15300000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="62"/>
+      <c r="B5" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="63">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="D5" s="63">
+        <v>91.650999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="62"/>
+      <c r="B6" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="63">
+        <v>1.052</v>
+      </c>
+      <c r="D6" s="63">
+        <v>80.709000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="62"/>
+      <c r="B7" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="63">
+        <v>1.006</v>
+      </c>
+      <c r="D7" s="63">
+        <v>112.214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="62"/>
+      <c r="B8" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="63">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D8" s="63">
+        <v>170.47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="62"/>
+      <c r="B9" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="C9" s="63">
+        <v>1</v>
+      </c>
+      <c r="D9" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="63">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="D10" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="80"/>
+      <c r="B11" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="C11" s="63">
+        <v>1.252</v>
+      </c>
+      <c r="D11" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="80"/>
+      <c r="B12" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="63">
+        <v>1.2130000000000001</v>
+      </c>
+      <c r="D12" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="80"/>
+      <c r="B13" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="35">
-        <v>0.308</v>
-      </c>
-      <c r="D3" s="35">
+      <c r="C13" s="63">
+        <v>1.25</v>
+      </c>
+      <c r="D13" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-      <c r="B4" s="36" t="s">
+    <row r="14" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="80"/>
+      <c r="B14" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="35">
-        <v>0.318</v>
-      </c>
-      <c r="D4" s="35">
+      <c r="C14" s="63">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="D14" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="B5" s="36" t="s">
+    <row r="15" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="80"/>
+      <c r="B15" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="35">
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="D5" s="35">
+      <c r="C15" s="63">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="D15" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="35">
-        <v>0.318</v>
-      </c>
-      <c r="D6" s="35">
+    <row r="16" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="80"/>
+      <c r="B16" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="63">
+        <v>1</v>
+      </c>
+      <c r="D16" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="B7" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="35">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="D7" s="35">
+    <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="63">
+        <v>1.141</v>
+      </c>
+      <c r="D17" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-      <c r="B8" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="35">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="D8" s="35">
+    <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="80"/>
+      <c r="B18" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="63">
+        <v>1.1739999999999999</v>
+      </c>
+      <c r="D18" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-      <c r="B9" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="35">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="D9" s="35">
+    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="80"/>
+      <c r="B19" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="63">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="D19" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="80"/>
+      <c r="B20" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="63">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="D20" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="80"/>
+      <c r="B21" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="63">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="D21" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="80"/>
+      <c r="B22" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="63">
+        <v>1.028</v>
+      </c>
+      <c r="D22" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="80"/>
+      <c r="B23" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="63">
+        <v>1</v>
+      </c>
+      <c r="D23" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B24" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="63">
+        <v>1.54</v>
+      </c>
+      <c r="D24" s="63">
+        <v>24.617000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="80"/>
+      <c r="B25" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="63">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="D25" s="63">
+        <v>28.425000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="80"/>
+      <c r="B26" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="63">
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="D26" s="63">
+        <v>25.533999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="80"/>
+      <c r="B27" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="35">
-        <v>0.373</v>
-      </c>
-      <c r="D10" s="35">
-        <v>24.617000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11"/>
-      <c r="B11" s="36" t="s">
+      <c r="C27" s="63">
+        <v>1.4670000000000001</v>
+      </c>
+      <c r="D27" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="80"/>
+      <c r="B28" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="35">
-        <v>0.4</v>
-      </c>
-      <c r="D11" s="35">
-        <v>28.425000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="B12" s="36" t="s">
+      <c r="C28" s="63">
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="D28" s="63">
+        <v>12.728</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="80"/>
+      <c r="B29" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="35">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="D12" s="35">
-        <v>25.533999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13"/>
-      <c r="B13" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="35">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="D13" s="35">
+      <c r="C29" s="63">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="D29" s="63">
+        <v>24.818999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="80"/>
+      <c r="B30" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="63">
+        <v>1</v>
+      </c>
+      <c r="D30" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14"/>
-      <c r="B14" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="35">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="D14" s="35">
-        <v>12.728</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15"/>
-      <c r="B15" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="35">
-        <v>0.59899999999999998</v>
-      </c>
-      <c r="D15" s="35">
-        <v>24.818999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="35">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="D16" s="35">
+    <row r="31" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="63">
+        <v>1.58</v>
+      </c>
+      <c r="D31" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+    <row r="32" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="80"/>
+      <c r="B32" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="63">
+        <v>1.506</v>
+      </c>
+      <c r="D32" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="80"/>
+      <c r="B33" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="C33" s="63">
+        <v>1.5229999999999999</v>
+      </c>
+      <c r="D33" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="80"/>
+      <c r="B34" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="35">
-        <v>2.4460000000000002</v>
-      </c>
-      <c r="D17" s="35">
+      <c r="C34" s="63">
+        <v>1.5429999999999999</v>
+      </c>
+      <c r="D34" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18"/>
-      <c r="B18" s="36" t="s">
+    <row r="35" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="80"/>
+      <c r="B35" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="35">
-        <v>2.379</v>
-      </c>
-      <c r="D18" s="35">
+      <c r="C35" s="63">
+        <v>1.234</v>
+      </c>
+      <c r="D35" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19"/>
-      <c r="B19" s="36" t="s">
+    <row r="36" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="80"/>
+      <c r="B36" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="35">
-        <v>3.3359999999999999</v>
-      </c>
-      <c r="D19" s="35">
+      <c r="C36" s="63">
+        <v>1.389</v>
+      </c>
+      <c r="D36" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20"/>
-      <c r="B20" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="35">
-        <v>2.9129999999999998</v>
-      </c>
-      <c r="D20" s="35">
+    <row r="37" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="80"/>
+      <c r="B37" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="63">
+        <v>1</v>
+      </c>
+      <c r="D37" s="63">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21"/>
-      <c r="B21" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="35">
-        <v>3.0910000000000002</v>
-      </c>
-      <c r="D21" s="35">
+      <c r="E37" s="66"/>
+    </row>
+    <row r="38" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="63">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="D38" s="63">
+        <v>117.49</v>
+      </c>
+      <c r="E38" s="66"/>
+    </row>
+    <row r="39" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="80"/>
+      <c r="B39" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="63">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="D39" s="63">
+        <v>85.37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="80"/>
+      <c r="B40" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="63">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="D40" s="63">
+        <v>20.199000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="80"/>
+      <c r="B41" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="63">
+        <v>0.97</v>
+      </c>
+      <c r="D41" s="63">
+        <v>112.84099999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="80"/>
+      <c r="B42" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="63">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="D42" s="63">
+        <v>99.76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="80"/>
+      <c r="B43" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="63">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="D43" s="63">
+        <v>27.056000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="80"/>
+      <c r="B44" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="63">
+        <v>1</v>
+      </c>
+      <c r="D44" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22"/>
-      <c r="B22" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="35">
-        <v>2.7170000000000001</v>
-      </c>
-      <c r="D22" s="35">
+    <row r="45" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="63">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="D45" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23"/>
-      <c r="B23" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="35">
-        <v>2.7930000000000001</v>
-      </c>
-      <c r="D23" s="35">
+    <row r="46" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="80"/>
+      <c r="B46" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="63">
+        <v>1.01</v>
+      </c>
+      <c r="D46" s="63">
+        <v>23.664000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="80"/>
+      <c r="B47" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="63">
+        <v>1.01</v>
+      </c>
+      <c r="D47" s="63">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="36" t="s">
+    <row r="48" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="80"/>
+      <c r="B48" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="35">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="D24" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25"/>
-      <c r="B25" s="36" t="s">
+      <c r="C48" s="63">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="D48" s="63">
+        <v>11.874000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="80"/>
+      <c r="B49" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="35">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="D25" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26"/>
-      <c r="B26" s="36" t="s">
+      <c r="C49" s="63">
+        <v>0.98</v>
+      </c>
+      <c r="D49" s="63">
+        <v>11.874000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="80"/>
+      <c r="B50" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="35">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="D26" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27"/>
-      <c r="B27" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="35">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="D27" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28"/>
-      <c r="B28" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="35">
-        <v>0.126</v>
-      </c>
-      <c r="D28" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29"/>
-      <c r="B29" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="35">
-        <v>0.112</v>
-      </c>
-      <c r="D29" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30"/>
-      <c r="B30" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="35">
-        <v>0.156</v>
-      </c>
-      <c r="D30" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="35">
-        <v>1.5880000000000001</v>
-      </c>
-      <c r="D31" s="35">
-        <v>117.49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32"/>
-      <c r="B32" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="35">
-        <v>1.591</v>
-      </c>
-      <c r="D32" s="35">
-        <v>85.37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33"/>
-      <c r="B33" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="35">
-        <v>1.595</v>
-      </c>
-      <c r="D33" s="35">
-        <v>20.199000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34"/>
-      <c r="B34" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="35">
-        <v>1.593</v>
-      </c>
-      <c r="D34" s="35">
-        <v>112.84099999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35"/>
-      <c r="B35" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="35">
-        <v>1.6160000000000001</v>
-      </c>
-      <c r="D35" s="35">
-        <v>99.76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36"/>
-      <c r="B36" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="35">
-        <v>1.643</v>
-      </c>
-      <c r="D36" s="35">
-        <v>27.056000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="37">
-        <v>1.546</v>
-      </c>
-      <c r="D37" s="37">
+      <c r="C50" s="63">
+        <v>0.754</v>
+      </c>
+      <c r="D50" s="63">
+        <v>16.248000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="65"/>
+      <c r="B51" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="65">
+        <v>1</v>
+      </c>
+      <c r="D51" s="65">
         <v>0</v>
       </c>
     </row>
@@ -2884,7 +3076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
@@ -4782,402 +4974,402 @@
       </c>
     </row>
     <row r="126" spans="1:5" s="6" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="59"/>
-      <c r="B126" s="60">
+      <c r="A126" s="56"/>
+      <c r="B126" s="57">
         <v>24</v>
       </c>
-      <c r="C126" s="61">
+      <c r="C126" s="58">
         <v>5917744.8439999996</v>
       </c>
-      <c r="D126" s="60">
+      <c r="D126" s="57">
         <v>443</v>
       </c>
-      <c r="E126" s="60">
+      <c r="E126" s="57">
         <v>4638</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="B127" s="60">
+      <c r="A127" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B127" s="57">
         <v>0</v>
       </c>
-      <c r="C127" s="61">
+      <c r="C127" s="58">
         <v>17568788.433699999</v>
       </c>
-      <c r="D127" s="63">
+      <c r="D127" s="60">
         <v>695</v>
       </c>
-      <c r="E127" s="63">
+      <c r="E127" s="60">
         <v>7320</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="51"/>
+      <c r="A128" s="48"/>
       <c r="B128" s="4">
         <v>1</v>
       </c>
-      <c r="C128" s="61">
+      <c r="C128" s="58">
         <v>17568345.515299998</v>
       </c>
-      <c r="D128" s="63">
+      <c r="D128" s="60">
         <v>710</v>
       </c>
-      <c r="E128" s="63">
+      <c r="E128" s="60">
         <v>7470</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="51"/>
+      <c r="A129" s="48"/>
       <c r="B129" s="4">
         <v>2</v>
       </c>
-      <c r="C129" s="61">
+      <c r="C129" s="58">
         <v>17567925.9791</v>
       </c>
-      <c r="D129" s="63">
+      <c r="D129" s="60">
         <v>709</v>
       </c>
-      <c r="E129" s="63">
+      <c r="E129" s="60">
         <v>7460</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="51"/>
+      <c r="A130" s="48"/>
       <c r="B130" s="4">
         <v>3</v>
       </c>
-      <c r="C130" s="61">
+      <c r="C130" s="58">
         <v>17568979.975200001</v>
       </c>
-      <c r="D130" s="63">
+      <c r="D130" s="60">
         <v>708</v>
       </c>
-      <c r="E130" s="63">
+      <c r="E130" s="60">
         <v>7450</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="51"/>
+      <c r="A131" s="48"/>
       <c r="B131" s="4">
         <v>4</v>
       </c>
-      <c r="C131" s="61">
+      <c r="C131" s="58">
         <v>17568105.775400002</v>
       </c>
-      <c r="D131" s="63">
+      <c r="D131" s="60">
         <v>723</v>
       </c>
-      <c r="E131" s="63">
+      <c r="E131" s="60">
         <v>7600</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="51"/>
+      <c r="A132" s="48"/>
       <c r="B132" s="4">
         <v>5</v>
       </c>
-      <c r="C132" s="61">
+      <c r="C132" s="58">
         <v>17567265.842700001</v>
       </c>
-      <c r="D132" s="63">
+      <c r="D132" s="60">
         <v>736</v>
       </c>
-      <c r="E132" s="63">
+      <c r="E132" s="60">
         <v>7730</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="51"/>
+      <c r="A133" s="48"/>
       <c r="B133" s="4">
         <v>6</v>
       </c>
-      <c r="C133" s="61">
+      <c r="C133" s="58">
         <v>17569197.895300001</v>
       </c>
-      <c r="D133" s="63">
+      <c r="D133" s="60">
         <v>700</v>
       </c>
-      <c r="E133" s="63">
+      <c r="E133" s="60">
         <v>7370</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="51"/>
+      <c r="A134" s="48"/>
       <c r="B134" s="4">
         <v>7</v>
       </c>
-      <c r="C134" s="61">
+      <c r="C134" s="58">
         <v>17568264.252900001</v>
       </c>
-      <c r="D134" s="63">
+      <c r="D134" s="60">
         <v>678</v>
       </c>
-      <c r="E134" s="63">
+      <c r="E134" s="60">
         <v>7150</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="51"/>
+      <c r="A135" s="48"/>
       <c r="B135" s="4">
         <v>8</v>
       </c>
-      <c r="C135" s="61">
+      <c r="C135" s="58">
         <v>17568470.5645</v>
       </c>
-      <c r="D135" s="63">
+      <c r="D135" s="60">
         <v>701</v>
       </c>
-      <c r="E135" s="63">
+      <c r="E135" s="60">
         <v>7380</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="51"/>
+      <c r="A136" s="48"/>
       <c r="B136" s="4">
         <v>9</v>
       </c>
-      <c r="C136" s="61">
+      <c r="C136" s="58">
         <v>17567358.417399999</v>
       </c>
-      <c r="D136" s="63">
+      <c r="D136" s="60">
         <v>744</v>
       </c>
-      <c r="E136" s="63">
+      <c r="E136" s="60">
         <v>7810</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="51"/>
+      <c r="A137" s="48"/>
       <c r="B137" s="4">
         <v>10</v>
       </c>
-      <c r="C137" s="61">
+      <c r="C137" s="58">
         <v>17567910.4683</v>
       </c>
-      <c r="D137" s="63">
+      <c r="D137" s="60">
         <v>714</v>
       </c>
-      <c r="E137" s="63">
+      <c r="E137" s="60">
         <v>7510</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="51"/>
+      <c r="A138" s="48"/>
       <c r="B138" s="4">
         <v>11</v>
       </c>
-      <c r="C138" s="61">
+      <c r="C138" s="58">
         <v>17567562.846000001</v>
       </c>
-      <c r="D138" s="63">
+      <c r="D138" s="60">
         <v>726</v>
       </c>
-      <c r="E138" s="63">
+      <c r="E138" s="60">
         <v>7630</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="51"/>
+      <c r="A139" s="48"/>
       <c r="B139" s="4">
         <v>12</v>
       </c>
-      <c r="C139" s="61">
+      <c r="C139" s="58">
         <v>17568503.699999999</v>
       </c>
-      <c r="D139" s="63">
+      <c r="D139" s="60">
         <v>726</v>
       </c>
-      <c r="E139" s="63">
+      <c r="E139" s="60">
         <v>7630</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="51"/>
+      <c r="A140" s="48"/>
       <c r="B140" s="4">
         <v>13</v>
       </c>
-      <c r="C140" s="61">
+      <c r="C140" s="58">
         <v>17568406.681699999</v>
       </c>
-      <c r="D140" s="63">
+      <c r="D140" s="60">
         <v>716</v>
       </c>
-      <c r="E140" s="63">
+      <c r="E140" s="60">
         <v>7530</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="51"/>
+      <c r="A141" s="48"/>
       <c r="B141" s="4">
         <v>14</v>
       </c>
-      <c r="C141" s="61">
+      <c r="C141" s="58">
         <v>17567663.021699999</v>
       </c>
-      <c r="D141" s="63">
+      <c r="D141" s="60">
         <v>703</v>
       </c>
-      <c r="E141" s="63">
+      <c r="E141" s="60">
         <v>7400</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="51"/>
+      <c r="A142" s="48"/>
       <c r="B142" s="4">
         <v>15</v>
       </c>
-      <c r="C142" s="61">
+      <c r="C142" s="58">
         <v>17567352.194699999</v>
       </c>
-      <c r="D142" s="63">
+      <c r="D142" s="60">
         <v>742</v>
       </c>
-      <c r="E142" s="63">
+      <c r="E142" s="60">
         <v>7790</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="51"/>
+      <c r="A143" s="48"/>
       <c r="B143" s="4">
         <v>16</v>
       </c>
-      <c r="C143" s="61">
+      <c r="C143" s="58">
         <v>17567777.249899998</v>
       </c>
-      <c r="D143" s="63">
+      <c r="D143" s="60">
         <v>729</v>
       </c>
-      <c r="E143" s="63">
+      <c r="E143" s="60">
         <v>7660</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="51"/>
+      <c r="A144" s="48"/>
       <c r="B144" s="4">
         <v>17</v>
       </c>
-      <c r="C144" s="61">
+      <c r="C144" s="58">
         <v>17568344.159899998</v>
       </c>
-      <c r="D144" s="63">
+      <c r="D144" s="60">
         <v>756</v>
       </c>
-      <c r="E144" s="63">
+      <c r="E144" s="60">
         <v>7930</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="51"/>
+      <c r="A145" s="48"/>
       <c r="B145" s="4">
         <v>18</v>
       </c>
-      <c r="C145" s="61">
+      <c r="C145" s="58">
         <v>17568257.8365</v>
       </c>
-      <c r="D145" s="63">
+      <c r="D145" s="60">
         <v>734</v>
       </c>
-      <c r="E145" s="63">
+      <c r="E145" s="60">
         <v>7710</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="51"/>
+      <c r="A146" s="48"/>
       <c r="B146" s="4">
         <v>19</v>
       </c>
-      <c r="C146" s="61">
+      <c r="C146" s="58">
         <v>17568103.004700001</v>
       </c>
-      <c r="D146" s="63">
+      <c r="D146" s="60">
         <v>712</v>
       </c>
-      <c r="E146" s="63">
+      <c r="E146" s="60">
         <v>7490</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="51"/>
+      <c r="A147" s="48"/>
       <c r="B147" s="4">
         <v>20</v>
       </c>
-      <c r="C147" s="61">
+      <c r="C147" s="58">
         <v>17567823.369100001</v>
       </c>
-      <c r="D147" s="63">
+      <c r="D147" s="60">
         <v>706</v>
       </c>
-      <c r="E147" s="63">
+      <c r="E147" s="60">
         <v>7430</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="51"/>
+      <c r="A148" s="48"/>
       <c r="B148" s="4">
         <v>21</v>
       </c>
-      <c r="C148" s="61">
+      <c r="C148" s="58">
         <v>17568645.069400001</v>
       </c>
-      <c r="D148" s="63">
+      <c r="D148" s="60">
         <v>733</v>
       </c>
-      <c r="E148" s="63">
+      <c r="E148" s="60">
         <v>7700</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="51"/>
+      <c r="A149" s="48"/>
       <c r="B149" s="4">
         <v>22</v>
       </c>
-      <c r="C149" s="61">
+      <c r="C149" s="58">
         <v>17568881.984000001</v>
       </c>
-      <c r="D149" s="63">
+      <c r="D149" s="60">
         <v>688</v>
       </c>
-      <c r="E149" s="63">
+      <c r="E149" s="60">
         <v>7250</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="51"/>
+      <c r="A150" s="48"/>
       <c r="B150" s="4">
         <v>23</v>
       </c>
-      <c r="C150" s="61">
+      <c r="C150" s="58">
         <v>17568584.1358</v>
       </c>
-      <c r="D150" s="63">
+      <c r="D150" s="60">
         <v>725</v>
       </c>
-      <c r="E150" s="63">
+      <c r="E150" s="60">
         <v>7620</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="59"/>
-      <c r="B151" s="60">
+      <c r="A151" s="56"/>
+      <c r="B151" s="57">
         <v>24</v>
       </c>
-      <c r="C151" s="61">
+      <c r="C151" s="58">
         <v>17568345.150800001</v>
       </c>
-      <c r="D151" s="63">
+      <c r="D151" s="60">
         <v>708</v>
       </c>
-      <c r="E151" s="63">
+      <c r="E151" s="60">
         <v>7450</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="B152" s="60">
+      <c r="A152" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="B152" s="57">
         <v>0</v>
       </c>
     </row>
@@ -5297,7 +5489,7 @@
       </c>
     </row>
     <row r="176" spans="2:2" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B176" s="60">
+      <c r="B176" s="57">
         <v>24</v>
       </c>
     </row>
@@ -5323,8 +5515,8 @@
   <sheetData>
     <row r="1" spans="1:12" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
       <c r="D1" s="28" t="s">
         <v>26</v>
       </c>
@@ -5341,51 +5533,51 @@
         <v>30</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" s="26" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="73"/>
+      <c r="A2" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:12" s="26" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="72"/>
+      <c r="A3" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="74"/>
     </row>
     <row r="4" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="30">
         <v>99.075109999999995</v>
@@ -5414,10 +5606,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="72"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="30">
         <v>181.7039</v>
@@ -5446,10 +5638,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="74"/>
-      <c r="B6" s="74"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="76"/>
       <c r="C6" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D6" s="30">
         <v>125.545</v>
@@ -5478,40 +5670,40 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="26" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="74"/>
+    </row>
+    <row r="8" spans="1:12" s="26" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="72"/>
-    </row>
-    <row r="8" spans="1:12" s="26" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="72"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="74"/>
     </row>
     <row r="9" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="72"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="30">
         <v>137.6952</v>
@@ -5540,10 +5732,10 @@
       </c>
     </row>
     <row r="10" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10" s="30">
         <v>125.9284</v>
@@ -5572,10 +5764,10 @@
       </c>
     </row>
     <row r="11" spans="1:12" s="26" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="74"/>
-      <c r="B11" s="74"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" s="30">
         <v>142.7004</v>
@@ -5604,40 +5796,40 @@
       </c>
     </row>
     <row r="12" spans="1:12" s="26" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="74"/>
+    </row>
+    <row r="13" spans="1:12" s="26" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="74"/>
+    </row>
+    <row r="14" spans="1:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="29" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="72"/>
-    </row>
-    <row r="13" spans="1:12" s="26" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="72"/>
-    </row>
-    <row r="14" spans="1:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="29" t="s">
-        <v>40</v>
       </c>
       <c r="D14" s="30">
         <v>99.706549999999993</v>
@@ -5666,10 +5858,10 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="72"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D15" s="30">
         <v>205</v>
@@ -5698,10 +5890,10 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="76"/>
+      <c r="A16" s="79"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D16" s="32">
         <v>101.46550000000001</v>
@@ -5749,8 +5941,6 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
@@ -5764,16 +5954,18 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>